<commit_message>
Update profit.py after running on 2025-08-20
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,16 @@
         <v>13493.98</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/20/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>13350.54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-21
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,16 @@
         <v>13350.54</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>08/21/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>13491.24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-23
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -1,64 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding_stuff\crypto_buys\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0A6FB6-09F8-4BBB-8616-4848497E4361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="2100" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Profit</t>
-  </si>
-  <si>
-    <t>08/19/2025</t>
-  </si>
-  <si>
-    <t>08/20/2025</t>
-  </si>
-  <si>
-    <t>08/21/2025</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -73,44 +49,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -398,56 +425,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/19/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>13493.98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/20/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>13350.54</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>08/21/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>13491.24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="3" t="n">
         <v>45891</v>
       </c>
-      <c r="B5">
-        <v>16663.080000000002</v>
+      <c r="B5" t="n">
+        <v>16663.08</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>08/23/2025</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>15810.39</v>
       </c>
     </row>
   </sheetData>
@@ -456,15 +504,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ECD0AD-268A-4B2A-ADF1-B9E80F232D83}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/23/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.09208987322815021</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9079101267718498</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-24
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -1,76 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding_stuff\crypto_buys\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BCD836-38FD-47C3-AD9A-A1FC43CC94DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Profit</t>
-  </si>
-  <si>
-    <t>08/19/2025</t>
-  </si>
-  <si>
-    <t>08/20/2025</t>
-  </si>
-  <si>
-    <t>08/21/2025</t>
-  </si>
-  <si>
-    <t>08/23/2025</t>
-  </si>
-  <si>
-    <t>BTC Allocation</t>
-  </si>
-  <si>
-    <t>Kaspa Allocation</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,44 +49,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -410,64 +425,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/19/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>13493.98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/20/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>13350.54</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>08/21/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>13491.24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="3" t="n">
         <v>45891</v>
       </c>
-      <c r="B5">
-        <v>16663.080000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+      <c r="B5" t="n">
+        <v>16663.08</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>08/23/2025</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>15810.39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>08/24/2025</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>15391.59</v>
       </c>
     </row>
   </sheetData>
@@ -476,39 +514,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>9.208987322815021E-2</v>
-      </c>
-      <c r="C2">
-        <v>0.90791012677184979</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/24/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.09522359804995995</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9047764019500401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-25
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,16 @@
       </c>
       <c r="B7" t="n">
         <v>15391.59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>08/25/2025</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>14927.67</v>
       </c>
     </row>
   </sheetData>
@@ -530,14 +540,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>08/24/2025</t>
+          <t>08/25/2025</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.09522359804995995</v>
+        <v>0.09453157997486517</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9047764019500401</v>
+        <v>0.9054684200251348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-26
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -1,82 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding_stuff\crypto_buys\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A50BD7-2324-4175-BAA1-54D9E17DB0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Profit</t>
-  </si>
-  <si>
-    <t>08/19/2025</t>
-  </si>
-  <si>
-    <t>08/20/2025</t>
-  </si>
-  <si>
-    <t>08/21/2025</t>
-  </si>
-  <si>
-    <t>08/23/2025</t>
-  </si>
-  <si>
-    <t>08/24/2025</t>
-  </si>
-  <si>
-    <t>08/25/2025</t>
-  </si>
-  <si>
-    <t>BTC %</t>
-  </si>
-  <si>
-    <t>KAS %</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -91,44 +49,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -416,80 +425,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/19/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>13493.98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/20/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>13350.54</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>08/21/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>13491.24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="3" t="n">
         <v>45891</v>
       </c>
-      <c r="B5">
-        <v>16663.080000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+      <c r="B5" t="n">
+        <v>16663.08</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>08/23/2025</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>15810.39</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>08/24/2025</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>15391.59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>08/25/2025</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>14927.67</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>08/26/2025</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>14690.84</v>
       </c>
     </row>
   </sheetData>
@@ -498,35 +534,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>9.4531579974865165E-2</v>
-      </c>
-      <c r="C2">
-        <v>0.90546842002513483</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/26/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.09467279385344451</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9053272061465555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-27
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -1,85 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding_stuff\crypto_buys\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FFB8F2-3F6D-4E27-B143-233F023985D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Profit</t>
-  </si>
-  <si>
-    <t>08/19/2025</t>
-  </si>
-  <si>
-    <t>08/20/2025</t>
-  </si>
-  <si>
-    <t>08/21/2025</t>
-  </si>
-  <si>
-    <t>08/23/2025</t>
-  </si>
-  <si>
-    <t>08/24/2025</t>
-  </si>
-  <si>
-    <t>08/25/2025</t>
-  </si>
-  <si>
-    <t>08/26/2025</t>
-  </si>
-  <si>
-    <t>BTC</t>
-  </si>
-  <si>
-    <t>KAS</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -94,44 +49,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -419,83 +425,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/19/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>13493.98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/20/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>13350.54</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>08/21/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>13491.24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="3" t="n">
         <v>45891</v>
       </c>
-      <c r="B5">
-        <v>16663.080000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+      <c r="B5" t="n">
+        <v>16663.08</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>08/23/2025</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>15810.39</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>08/24/2025</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>15391.59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>08/25/2025</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>14927.67</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>08/26/2025</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>14690.84</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>08/27/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>14964.71</v>
       </c>
     </row>
   </sheetData>
@@ -504,35 +544,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>9.4672793853444515E-2</v>
-      </c>
-      <c r="C2">
-        <v>0.90532720614655549</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>08/27/2025</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>0.09399827411551842</v>
+      </c>
+      <c r="C1" t="n">
+        <v>0.9060017258844816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-28
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,16 @@
       </c>
       <c r="B10" t="n">
         <v>14964.71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>08/28/2025</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>15832.36</v>
       </c>
     </row>
   </sheetData>
@@ -560,14 +570,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>08/27/2025</t>
+          <t>08/28/2025</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.09399827411551842</v>
+        <v>0.09439885811184578</v>
       </c>
       <c r="C1" t="n">
-        <v>0.9060017258844816</v>
+        <v>0.9056011418881542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-29
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,6 +546,16 @@
       </c>
       <c r="B11" t="n">
         <v>15832.36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>08/29/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>11839.93</v>
       </c>
     </row>
   </sheetData>
@@ -570,14 +580,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>08/28/2025</t>
+          <t>08/29/2025</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.09439885811184578</v>
+        <v>0.1104204078508326</v>
       </c>
       <c r="C1" t="n">
-        <v>0.9056011418881542</v>
+        <v>0.8895795921491674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-30
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,16 @@
       </c>
       <c r="B12" t="n">
         <v>11839.93</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08/30/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>11447.83</v>
       </c>
     </row>
   </sheetData>
@@ -580,14 +590,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>08/29/2025</t>
+          <t>08/30/2025</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.1104204078508326</v>
+        <v>0.1105078176324462</v>
       </c>
       <c r="C1" t="n">
-        <v>0.8895795921491674</v>
+        <v>0.8894921823675538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-08-31
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,6 +566,16 @@
       </c>
       <c r="B13" t="n">
         <v>11447.83</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>08/31/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>11540.15</v>
       </c>
     </row>
   </sheetData>
@@ -590,14 +600,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>08/30/2025</t>
+          <t>08/31/2025</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.1105078176324462</v>
+        <v>0.1124501629923415</v>
       </c>
       <c r="C1" t="n">
-        <v>0.8894921823675538</v>
+        <v>0.8875498370076585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-09-01
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,6 +576,16 @@
       </c>
       <c r="B14" t="n">
         <v>11540.15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>09/01/2025</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>11390.83</v>
       </c>
     </row>
   </sheetData>
@@ -600,14 +610,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>08/31/2025</t>
+          <t>09/01/2025</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.1124501629923415</v>
+        <v>0.1138573803187714</v>
       </c>
       <c r="C1" t="n">
-        <v>0.8875498370076585</v>
+        <v>0.8861426196812286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit.py after running on 2025-09-02
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -430,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +480,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="2" t="n">
         <v>45891</v>
       </c>
       <c r="B5" t="n">
@@ -588,36 +587,14 @@
         <v>11390.83</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>09/01/2025</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>0.1138573803187714</v>
-      </c>
-      <c r="C1" t="n">
-        <v>0.8861426196812286</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>09/02/2025</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>13336.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-03
</commit_message>
<xml_diff>
--- a/data/profit.xlsx
+++ b/data/profit.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,6 +597,16 @@
         <v>13336.21</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>09/03/2025</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>13755.16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>